<commit_message>
Temporarily add the xl
</commit_message>
<xml_diff>
--- a/articles/iot-hub/iot-hub-metrics-table.xlsx
+++ b/articles/iot-hub/iot-hub-metrics-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\azure-docs-pr\articles\iot-hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F28225-AE20-4D74-A900-5484A62B9E37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FB9B79-9A97-4820-8BC1-DFB597EBE10A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25320" yWindow="-15240" windowWidth="18225" windowHeight="11535" xr2:uid="{4D434432-2D31-4BF1-9354-EEB50D7CB4FE}"/>
+    <workbookView xWindow="-2865" yWindow="-15015" windowWidth="18225" windowHeight="11535" xr2:uid="{4D434432-2D31-4BF1-9354-EEB50D7CB4FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -762,12 +762,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -777,6 +771,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1095,7 +1095,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA7FFFD-ACC2-4C80-8CE9-66F756DD8860}">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1167,23 +1169,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="7" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
@@ -1265,7 +1267,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1305,7 +1307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="242.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -1325,7 +1327,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -1364,7 +1366,7 @@
       <c r="F13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="6" t="s">
         <v>212</v>
       </c>
     </row>
@@ -1387,11 +1389,11 @@
       <c r="F14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -1411,7 +1413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
@@ -1431,7 +1433,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -1450,7 +1452,7 @@
       <c r="F17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="6" t="s">
         <v>214</v>
       </c>
     </row>
@@ -1474,7 +1476,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="114" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>59</v>
       </c>
@@ -1514,7 +1516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>65</v>
       </c>
@@ -1533,11 +1535,11 @@
       <c r="F21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
@@ -1557,7 +1559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="114" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>71</v>
       </c>
@@ -1577,7 +1579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>74</v>
       </c>
@@ -1597,7 +1599,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>77</v>
       </c>
@@ -1617,7 +1619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>80</v>
       </c>
@@ -1658,62 +1660,62 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="178.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="5" t="s">
+      <c r="C28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>89</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="7" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="224.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="8" t="s">
         <v>95</v>
       </c>
       <c r="F31" s="2" t="s">
@@ -1721,11 +1723,11 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
       <c r="F32" s="2" t="s">
         <v>92</v>
       </c>
@@ -1770,7 +1772,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>102</v>
       </c>
@@ -1790,7 +1792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>105</v>
       </c>
@@ -1849,7 +1851,7 @@
       <c r="F38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G38" s="6" t="s">
         <v>217</v>
       </c>
     </row>
@@ -1872,7 +1874,7 @@
       <c r="F39" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G39" s="8"/>
+      <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
@@ -1913,7 +1915,7 @@
       <c r="F41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="G41" s="6" t="s">
         <v>217</v>
       </c>
     </row>
@@ -1936,7 +1938,7 @@
       <c r="F42" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" s="6" t="s">
         <v>217</v>
       </c>
     </row>
@@ -1999,11 +2001,11 @@
       <c r="F45" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="G45" s="6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>135</v>
       </c>
@@ -2062,11 +2064,11 @@
       <c r="F48" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G48" s="6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>144</v>
       </c>
@@ -2125,7 +2127,7 @@
       <c r="F51" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="G51" s="6" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2249,7 +2251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>171</v>
       </c>
@@ -2289,7 +2291,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>177</v>
       </c>
@@ -2349,7 +2351,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>186</v>
       </c>
@@ -2389,7 +2391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>192</v>
       </c>
@@ -2409,7 +2411,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>195</v>
       </c>
@@ -2452,7 +2454,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>200</v>
       </c>
@@ -2514,16 +2516,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="E28:E30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:E32"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="E28:E30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E28" r:id="rId1" display="https://aka.ms/ioteventgrid" xr:uid="{CB44FAD1-7389-4ADC-9B0D-B6676BC5F4A0}"/>

</xml_diff>